<commit_message>
Updated R7 report, updated summed time
Kim has not yet reported time for R7 and the report must be updated to
reflect this.
</commit_message>
<xml_diff>
--- a/Docs/R7 numbers.xlsx
+++ b/Docs/R7 numbers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -481,11 +481,14 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
@@ -523,7 +526,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.5</c:v>
@@ -547,24 +550,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="82522112"/>
-        <c:axId val="82523648"/>
+        <c:axId val="161458048"/>
+        <c:axId val="161459584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82522112"/>
+        <c:axId val="161458048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82523648"/>
+        <c:crossAx val="161459584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82523648"/>
+        <c:axId val="161459584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,7 +575,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82522112"/>
+        <c:crossAx val="161458048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -585,7 +588,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -646,7 +649,7 @@
                   <c:v>5575</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7271</c:v>
+                  <c:v>7404</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -699,31 +702,31 @@
                   <c:v>3356</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3886</c:v>
+                  <c:v>3975</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82662528"/>
-        <c:axId val="82664064"/>
+        <c:axId val="161475584"/>
+        <c:axId val="161923840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82662528"/>
+        <c:axId val="161475584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82664064"/>
+        <c:crossAx val="161923840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82664064"/>
+        <c:axId val="161923840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,7 +734,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82662528"/>
+        <c:crossAx val="161475584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -744,7 +747,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1194,24 +1197,24 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="83237120"/>
-        <c:axId val="83251200"/>
+        <c:axId val="163419264"/>
+        <c:axId val="163420800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83237120"/>
+        <c:axId val="163419264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83251200"/>
+        <c:crossAx val="163420800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83251200"/>
+        <c:axId val="163420800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1219,7 +1222,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83237120"/>
+        <c:crossAx val="163419264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1232,7 +1235,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1631,7 +1634,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C21"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1648,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1689,7 +1692,7 @@
         <v>40</v>
       </c>
       <c r="E30">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="3:5">
@@ -1710,6 +1713,9 @@
       <c r="D32">
         <v>5</v>
       </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="3:5">
       <c r="C33" t="s">
@@ -1859,7 +1865,7 @@
         <v>2</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="3:5">
@@ -1938,8 +1944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1979,10 +1985,10 @@
         <v>36</v>
       </c>
       <c r="D5">
-        <v>7271</v>
+        <v>7404</v>
       </c>
       <c r="E5">
-        <v>3886</v>
+        <v>3975</v>
       </c>
     </row>
   </sheetData>
@@ -1995,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>